<commit_message>
better formatting for xlsx file
</commit_message>
<xml_diff>
--- a/backend/api/v1/streams/templates/StreamApportionment.xlsx
+++ b/backend/api/v1/streams/templates/StreamApportionment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephhil/devel/wally/backend/api/v1/streams/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA33D8A6-E105-1849-8677-46174BFE22DE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D483BE7-E93B-0D46-9378-470EFDE627E4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{DE171BF9-B95D-114C-BEF9-BD9A0898B691}"/>
+    <workbookView xWindow="2400" yWindow="740" windowWidth="33600" windowHeight="20540" xr2:uid="{DE171BF9-B95D-114C-BEF9-BD9A0898B691}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,23 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Stream apportionment</t>
   </si>
   <si>
-    <t xml:space="preserve">Generated: </t>
-  </si>
-  <si>
-    <t>Streams</t>
-  </si>
-  <si>
-    <t>Point of interest: {d.point}</t>
-  </si>
-  <si>
-    <t>Weighting factor: {d.weighting_factor}</t>
-  </si>
-  <si>
     <t>{d.streams[i].gnis_name}</t>
   </si>
   <si>
@@ -61,13 +49,34 @@
   </si>
   <si>
     <t>Apportionment (%)</t>
+  </si>
+  <si>
+    <t>Point of interest:</t>
+  </si>
+  <si>
+    <t>{d.point}</t>
+  </si>
+  <si>
+    <t>Weighting factor:</t>
+  </si>
+  <si>
+    <t>{d.weighting_factor}</t>
+  </si>
+  <si>
+    <t>GNIS Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date generated: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,6 +88,14 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,9 +131,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -133,6 +151,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD352918-ACC0-CC42-AF80-AD9F76F2AC88}" name="Table1" displayName="Table1" ref="A6:C8" totalsRowShown="0">
+  <autoFilter ref="A6:C8" xr:uid="{3C13AB81-976B-5241-8914-F3E485641973}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{3168EC2B-7CDF-404E-9142-C4B6D450497C}" name="GNIS Name"/>
+    <tableColumn id="2" xr3:uid="{322D25D9-540F-5E4E-A4FC-5ED2A43AFA07}" name="Distance (m)"/>
+    <tableColumn id="3" xr3:uid="{798C52E9-E667-134D-B82E-C1794B40E879}" name="Apportionment (%)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,15 +462,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4329F68-75D9-CE41-906C-55BAAEE40BCD}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -452,52 +484,66 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add length to excel sheet
</commit_message>
<xml_diff>
--- a/backend/api/v1/streams/templates/StreamApportionment.xlsx
+++ b/backend/api/v1/streams/templates/StreamApportionment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephhil/devel/wally/backend/api/v1/streams/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC31EB74-A703-9A4C-9A74-22B8572E1744}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DBE5AD-A7F8-BA46-B64A-D2916EA6DEFE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="740" windowWidth="33600" windowHeight="20540" xr2:uid="{DE171BF9-B95D-114C-BEF9-BD9A0898B691}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Stream apportionment</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Length of reach (m)</t>
+  </si>
+  <si>
+    <t>{d.streams[i].length_metre}</t>
   </si>
 </sst>
 </file>
@@ -501,14 +507,15 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -516,8 +523,6 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -553,9 +558,12 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -564,9 +572,12 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>